<commit_message>
updated version with excel
</commit_message>
<xml_diff>
--- a/base.xlsx
+++ b/base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aluno TDS\Documents\git-paulo\uc10_notas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2B644420-2295-4AC8-BD3B-05E4106FC72A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7442BAA-EA80-446C-B352-CFE3D613D777}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{040A00F2-F429-431E-AE6E-13C3D58AFC8A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Student</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>Kainna</t>
+  </si>
+  <si>
+    <t>Grade3</t>
+  </si>
+  <si>
+    <t>Tymotheo</t>
   </si>
 </sst>
 </file>
@@ -61,12 +67,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -81,8 +99,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,57 +425,122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0F0508F-3956-4A39-AC57-3578888CED0D}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="3">
         <v>5</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="E2" s="3">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>7</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <v>3</v>
       </c>
+      <c r="E3" s="3">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3">
+        <v>4</v>
+      </c>
+      <c r="D4" s="3">
+        <v>4</v>
+      </c>
+      <c r="E4" s="3">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F8" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>